<commit_message>
minor update for calibration curve - remove space in hmdbid
</commit_message>
<xml_diff>
--- a/lib/APGCMS/APGCMS/lib/lib_urine_CalibrationCurve_TropicAcid_20170823.xlsx
+++ b/lib/APGCMS/APGCMS/lib/lib_urine_CalibrationCurve_TropicAcid_20170823.xlsx
@@ -561,9 +561,6 @@
     <t>2-Hydroxy-2-methylbutyric acid</t>
   </si>
   <si>
-    <t xml:space="preserve">HMDB00115 </t>
-  </si>
-  <si>
     <t>Glycolic acid</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>2-methylmalic</t>
+  </si>
+  <si>
+    <t>HMDB00115</t>
   </si>
 </sst>
 </file>
@@ -1433,7 +1433,7 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1527,10 +1527,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>178</v>
       </c>
       <c r="D3" s="9">
         <v>6</v>
@@ -2179,10 +2179,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>182</v>
       </c>
       <c r="D21" s="9">
         <v>1</v>
@@ -2401,10 +2401,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>184</v>
       </c>
       <c r="D27" s="9">
         <v>2</v>
@@ -2614,10 +2614,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="D33" s="9">
         <v>2</v>
@@ -3855,10 +3855,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="D67" s="9">
         <v>2</v>
@@ -4290,10 +4290,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>180</v>
       </c>
       <c r="D79" s="9">
         <v>1</v>

</xml_diff>